<commit_message>
added identifiable example email addresses to the example data
</commit_message>
<xml_diff>
--- a/example_week.xlsx
+++ b/example_week.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\falbers\OneDrive - MathWorks\Documents\MATLAB\ProjectsToGit\FileExchange_MATLABGraderGradebook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\falbers\OneDrive - MathWorks\Documents\MATLAB\ProjectsToGit\Gitlab_CustomizableAssignmentReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{5F78753B-4286-4E29-8528-074BD23C84B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{93A4821F-13FE-44B0-9F4E-2AFC46452CB4}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{5F78753B-4286-4E29-8528-074BD23C84B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6FF51C52-BC02-41C4-B568-1F4011DC0838}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
   <si>
     <t>Student Name</t>
   </si>
@@ -215,10 +215,7 @@
     <t>2021-05-12 11:33:09 CEST</t>
   </si>
   <si>
-    <t>examplemail</t>
-  </si>
-  <si>
-    <t>Sebastian</t>
+    <t xml:space="preserve">Sebastian </t>
   </si>
   <si>
     <t xml:space="preserve">Jeff </t>
@@ -233,13 +230,37 @@
     <t xml:space="preserve">Spandhana </t>
   </si>
   <si>
+    <t>Stefan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Franziska </t>
+  </si>
+  <si>
     <t xml:space="preserve">Stefan </t>
   </si>
   <si>
-    <t xml:space="preserve">Franziska </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sebastian </t>
+    <t>Franziska</t>
+  </si>
+  <si>
+    <t>examplemail1</t>
+  </si>
+  <si>
+    <t>examplemail2</t>
+  </si>
+  <si>
+    <t>examplemail3</t>
+  </si>
+  <si>
+    <t>examplemail4</t>
+  </si>
+  <si>
+    <t>examplemail5</t>
+  </si>
+  <si>
+    <t>examplemail6</t>
+  </si>
+  <si>
+    <t>examplemail7</t>
   </si>
 </sst>
 </file>
@@ -592,7 +613,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -670,10 +691,10 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>68519422</v>
@@ -723,10 +744,10 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>68135571</v>
@@ -776,10 +797,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>68112791</v>
@@ -829,10 +850,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C5">
         <v>68154756</v>
@@ -882,10 +903,10 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C6">
         <v>66874397</v>
@@ -935,10 +956,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C7">
         <v>68116986</v>
@@ -988,10 +1009,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="C8">
         <v>72483140</v>
@@ -1041,10 +1062,10 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C9">
         <v>72689843</v>
@@ -1094,10 +1115,10 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C10">
         <v>72688593</v>
@@ -1147,10 +1168,10 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="C11">
         <v>72483200</v>
@@ -1204,6 +1225,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100980BDDEF46FE204DAE282A36E1D18E3A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5c5b9ea82e4fb2236a680405a4b70170">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f70b4450-89be-4009-afce-64b7a17b1b3f" xmlns:ns4="7c549c0e-d443-449d-9ea7-3b022ddbd72d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c716c87f0099c82efed9bb73d9fee0d0" ns3:_="" ns4:_="">
     <xsd:import namespace="f70b4450-89be-4009-afce-64b7a17b1b3f"/>
@@ -1420,22 +1456,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFE49873-FADB-4595-8C35-4DA6E919D713}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35736490-6787-420D-8F2A-2DC8D1367F1C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE695F08-BCE3-469E-B90B-911164892CB9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1452,21 +1490,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35736490-6787-420D-8F2A-2DC8D1367F1C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFE49873-FADB-4595-8C35-4DA6E919D713}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>